<commit_message>
Fix data less than template bug Change validate to validate_list
</commit_message>
<xml_diff>
--- a/test/t2_template.xlsx
+++ b/test/t2_template.xlsx
@@ -177,7 +177,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{{link1|validate('a,b,c')}}</t>
+    <t>{{link1|validate_list('a,b,c')}}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -936,7 +936,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>